<commit_message>
added few lines for visualization which needs to be cleaned up. This version of code does calibrate the model to the data presented by ICMR
</commit_message>
<xml_diff>
--- a/rate_matrix_old.xlsx
+++ b/rate_matrix_old.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijetadeshpande/Documents/GitHub/compartmental-model-COVID19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05686914-D43F-3343-9278-DFCED5673A3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9864A3CD-804E-4947-AAD0-D9FD77094135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{68BC5988-E0E2-3145-9802-2A71AB6DCC1D}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>&lt;60</t>
   </si>
   <si>
-    <t>exposed</t>
-  </si>
-  <si>
     <t>symptomatic</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>births</t>
+  </si>
+  <si>
+    <t>asymptomatic</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -541,33 +541,33 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
-      </c>
-      <c r="I1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>-1</v>
@@ -578,15 +578,15 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B3">
-        <f>(2.2/(11-2.5))</f>
-        <v>0.25882352941176473</v>
+        <f>(3.2/(11.5-2.5))</f>
+        <v>0.35555555555555557</v>
       </c>
       <c r="C3" s="1">
         <f>-SUM(D3:I3)</f>
-        <v>-9.1122993794526638E-2</v>
+        <v>-9.0909090909090912E-2</v>
       </c>
       <c r="D3" s="1">
         <f>1/11</f>
@@ -597,17 +597,16 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="10">
-        <f>(0.8*(1/(68.5*52*7)))+(0.2*0.02*1/22)</f>
-        <v>2.1390288543573217E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <f>(2.2/(11-2.5))</f>
-        <v>0.25882352941176473</v>
+        <f>(3.2/(11.5-2.5))</f>
+        <v>0.35555555555555557</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
@@ -616,46 +615,43 @@
       </c>
       <c r="E4" s="10">
         <f>1-SUM(F4:I4)</f>
-        <v>0.94264323997170707</v>
+        <v>1</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10">
-        <f>0.8*(1/14)</f>
-        <v>5.7142857142857141E-2</v>
+        <v>0</v>
       </c>
       <c r="I4" s="10">
-        <f>(0.8*(1/(68.5*52*7)))+(0.2*0.02*1/22)</f>
-        <v>2.1390288543573217E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="10">
         <f>-SUM(F5:H5)</f>
-        <v>-0.10571428571428571</v>
+        <v>-4.8571428571428571E-2</v>
       </c>
       <c r="F5" s="10">
         <f xml:space="preserve"> 0.2*(1/7)</f>
         <v>2.8571428571428571E-2</v>
       </c>
       <c r="G5" s="10">
-        <f>0.2*1/10</f>
-        <v>0.02</v>
+        <f>0.2*(1/10)</f>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="H5" s="10">
-        <f>0.8*(1/14)</f>
-        <v>5.7142857142857141E-2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -673,7 +669,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -694,7 +690,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -702,17 +698,15 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1">
-        <f>-I8</f>
-        <v>-4.0105879521937915E-5</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
-        <f>1/(68.5*52*7)</f>
-        <v>4.0105879521937915E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9">
         <v>0</v>

</xml_diff>